<commit_message>
Remove outdated scripts for generating LPU datasets and realistic budget samples
</commit_message>
<xml_diff>
--- a/data/inputs/lpu/BASE_LPU.xlsx
+++ b/data/inputs/lpu/BASE_LPU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emers\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e66243f108409f2/Área de Trabalho/Itaú/CICF/DataCraft/Verificador Inteligente de Obras/codes/construct-cost-ai/data/inputs/lpu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73562A5-4272-4DF6-8199-AAA8434F95BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D73562A5-4272-4DF6-8199-AAA8434F95BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FB803F4-2DD1-4241-9AC1-70A47138F4FE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5579,9 +5579,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>Un</t>
-  </si>
-  <si>
     <t>CENTRO-OESTE/NORDESTE-GRUPO1</t>
   </si>
   <si>
@@ -5613,6 +5610,9 @@
   </si>
   <si>
     <t>MULTIPLICADOR_BASE</t>
+  </si>
+  <si>
+    <t>Unid.</t>
   </si>
 </sst>
 </file>
@@ -5704,7 +5704,7 @@
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Cód Item"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Item"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Un"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Unid."/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="CENTRO-OESTE/NORDESTE-GRUPO1"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CENTRO-OESTE/NORDESTE-GRUPO2"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="CENTRO-OESTE/NORDESTE-GRUPO3"/>
@@ -6027,34 +6027,34 @@
         <v>1851</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>1863</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1852</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1853</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1854</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>1855</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1856</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1857</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>1858</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1859</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1860</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1861</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -44079,15 +44079,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1862</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1863</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -44095,7 +44095,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B3" s="4">
         <v>1.05</v>
@@ -44103,7 +44103,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B4" s="4">
         <v>1.1000000000000001</v>
@@ -44111,7 +44111,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B5" s="4">
         <v>1.08</v>
@@ -44119,7 +44119,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B6" s="4">
         <v>1.1299999999999999</v>
@@ -44127,7 +44127,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B7" s="4">
         <v>1.18</v>
@@ -44135,7 +44135,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B8" s="4">
         <v>0.97</v>
@@ -44143,7 +44143,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="B9" s="4">
         <v>1.02</v>
@@ -44151,7 +44151,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="B10" s="4">
         <v>1.07</v>

</xml_diff>

<commit_message>
feat: update LPU and NLPU validators with new output settings and data processing enhancements
</commit_message>
<xml_diff>
--- a/data/inputs/lpu/BASE_LPU.xlsx
+++ b/data/inputs/lpu/BASE_LPU.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -5696,6 +5696,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6008,7 +6012,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>